<commit_message>
he corregido un error en los periodos y he hecho un t-test para lswi y ndvi
</commit_message>
<xml_diff>
--- a/Excel/LSWI_zones_hum_buf.xlsx
+++ b/Excel/LSWI_zones_hum_buf.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6207" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6207" uniqueCount="88">
   <si>
     <t>wetland</t>
   </si>
@@ -300,60 +300,6 @@
   </si>
   <si>
     <t>2011_2021</t>
-  </si>
-  <si>
-    <t>1999_2011</t>
-  </si>
-  <si>
-    <t>2011_2022</t>
-  </si>
-  <si>
-    <t>1999_2012</t>
-  </si>
-  <si>
-    <t>2011_2023</t>
-  </si>
-  <si>
-    <t>1999_2013</t>
-  </si>
-  <si>
-    <t>2011_2024</t>
-  </si>
-  <si>
-    <t>1999_2014</t>
-  </si>
-  <si>
-    <t>2011_2025</t>
-  </si>
-  <si>
-    <t>1999_2015</t>
-  </si>
-  <si>
-    <t>2011_2026</t>
-  </si>
-  <si>
-    <t>1999_2016</t>
-  </si>
-  <si>
-    <t>2011_2027</t>
-  </si>
-  <si>
-    <t>1999_2017</t>
-  </si>
-  <si>
-    <t>2011_2028</t>
-  </si>
-  <si>
-    <t>1999_2018</t>
-  </si>
-  <si>
-    <t>2011_2029</t>
-  </si>
-  <si>
-    <t>1999_2019</t>
-  </si>
-  <si>
-    <t>2011_2030</t>
   </si>
   <si>
     <t>ndvi</t>
@@ -5797,7 +5743,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
         <v>23</v>
@@ -36555,7 +36501,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36601,7 +36547,7 @@
         <v>82</v>
       </c>
       <c r="N1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -36903,7 +36849,7 @@
         <v>54</v>
       </c>
       <c r="L8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M8">
         <v>5.9435603837133442E-2</v>
@@ -36947,7 +36893,7 @@
         <v>54</v>
       </c>
       <c r="L9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M9">
         <v>6.9642314837526836E-2</v>
@@ -36991,7 +36937,7 @@
         <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M10">
         <v>2.5071944804283524E-2</v>
@@ -37035,7 +36981,7 @@
         <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M11">
         <v>3.1126983130033814E-2</v>
@@ -37079,7 +37025,7 @@
         <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M12">
         <v>6.0217234087866977E-3</v>
@@ -37123,7 +37069,7 @@
         <v>46</v>
       </c>
       <c r="L13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M13">
         <v>8.1082019645145054E-3</v>
@@ -37167,7 +37113,7 @@
         <v>52</v>
       </c>
       <c r="L14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M14">
         <v>2.5665645987964975E-2</v>
@@ -37211,7 +37157,7 @@
         <v>52</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M15">
         <v>2.769231736851149E-2</v>
@@ -37255,7 +37201,7 @@
         <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M16">
         <v>1.4938913791498157E-2</v>
@@ -37299,7 +37245,7 @@
         <v>38</v>
       </c>
       <c r="L17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M17">
         <v>2.7099704482693155E-2</v>
@@ -37343,7 +37289,7 @@
         <v>36</v>
       </c>
       <c r="L18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M18">
         <v>-9.904844182702017E-4</v>
@@ -37387,7 +37333,7 @@
         <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M19">
         <v>7.9770028243829477E-3</v>
@@ -37431,7 +37377,7 @@
         <v>48</v>
       </c>
       <c r="L20" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M20">
         <v>2.5642564824018582E-2</v>
@@ -37475,7 +37421,7 @@
         <v>48</v>
       </c>
       <c r="L21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M21">
         <v>2.5051966761243848E-2</v>
@@ -37519,7 +37465,7 @@
         <v>56</v>
       </c>
       <c r="L22" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M22">
         <v>9.7797661960327535E-4</v>
@@ -37563,7 +37509,7 @@
         <v>56</v>
       </c>
       <c r="L23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M23">
         <v>1.6207627629022853E-2</v>
@@ -37607,7 +37553,7 @@
         <v>34</v>
       </c>
       <c r="L24" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M24">
         <v>-7.08161502297698E-3</v>
@@ -37651,7 +37597,7 @@
         <v>34</v>
       </c>
       <c r="L25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M25">
         <v>-4.8932573492571517E-3</v>
@@ -37695,7 +37641,7 @@
         <v>60</v>
       </c>
       <c r="L26" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M26">
         <v>-1.2461600626775128E-2</v>
@@ -37739,7 +37685,7 @@
         <v>60</v>
       </c>
       <c r="L27" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M27">
         <v>4.5052253859944906E-3</v>
@@ -37783,7 +37729,7 @@
         <v>40</v>
       </c>
       <c r="L28" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M28">
         <v>-2.0039932457807845E-3</v>
@@ -37827,7 +37773,7 @@
         <v>40</v>
       </c>
       <c r="L29" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M29">
         <v>3.9958162511490114E-3</v>
@@ -37871,7 +37817,7 @@
         <v>58</v>
       </c>
       <c r="L30" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="M30">
         <v>4.1730567105887573E-2</v>
@@ -37915,7 +37861,7 @@
         <v>58</v>
       </c>
       <c r="L31" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="M31">
         <v>5.727322563454116E-2</v>
@@ -37959,7 +37905,7 @@
         <v>44</v>
       </c>
       <c r="L32" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="M32">
         <v>8.7090621548857813E-2</v>
@@ -38003,7 +37949,7 @@
         <v>44</v>
       </c>
       <c r="L33" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="M33">
         <v>9.4676978535346304E-2</v>
@@ -38047,7 +37993,7 @@
         <v>42</v>
       </c>
       <c r="L34" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="M34">
         <v>4.2469476770690941E-2</v>
@@ -38091,7 +38037,7 @@
         <v>42</v>
       </c>
       <c r="L35" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="M35">
         <v>4.141994670177946E-2</v>
@@ -38135,7 +38081,7 @@
         <v>50</v>
       </c>
       <c r="L36" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="M36">
         <v>2.132641499793067E-3</v>
@@ -38179,7 +38125,7 @@
         <v>50</v>
       </c>
       <c r="L37" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="M37">
         <v>-1.7166748266250157E-4</v>
@@ -38223,7 +38169,7 @@
         <v>54</v>
       </c>
       <c r="L38" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="M38">
         <v>4.9487794229461674E-2</v>
@@ -38267,7 +38213,7 @@
         <v>54</v>
       </c>
       <c r="L39" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M39">
         <v>4.7710178476332167E-2</v>
@@ -38311,7 +38257,7 @@
         <v>62</v>
       </c>
       <c r="L40" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="M40">
         <v>5.5795264453984035E-2</v>
@@ -38355,7 +38301,7 @@
         <v>62</v>
       </c>
       <c r="L41" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M41">
         <v>6.7301898106033195E-2</v>
@@ -38399,7 +38345,7 @@
         <v>46</v>
       </c>
       <c r="L42" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="M42">
         <v>5.863461614124655E-2</v>
@@ -38443,7 +38389,7 @@
         <v>46</v>
       </c>
       <c r="L43" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="M43">
         <v>3.6829164110967413E-2</v>
@@ -38487,7 +38433,7 @@
         <v>52</v>
       </c>
       <c r="L44" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M44">
         <v>3.8684908059838659E-2</v>
@@ -38531,7 +38477,7 @@
         <v>52</v>
       </c>
       <c r="L45" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="M45">
         <v>3.5376219552520544E-2</v>
@@ -38575,7 +38521,7 @@
         <v>38</v>
       </c>
       <c r="L46" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M46">
         <v>3.2207712164394685E-2</v>
@@ -38619,7 +38565,7 @@
         <v>38</v>
       </c>
       <c r="L47" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="M47">
         <v>3.5757958146344242E-2</v>
@@ -38663,7 +38609,7 @@
         <v>36</v>
       </c>
       <c r="L48" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="M48">
         <v>8.2414019133299279E-2</v>
@@ -38707,7 +38653,7 @@
         <v>36</v>
       </c>
       <c r="L49" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="M49">
         <v>7.5054230434128275E-2</v>
@@ -38751,7 +38697,7 @@
         <v>48</v>
       </c>
       <c r="L50" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="M50">
         <v>5.0986036914478727E-2</v>
@@ -38795,7 +38741,7 @@
         <v>48</v>
       </c>
       <c r="L51" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="M51">
         <v>6.0172699135778385E-2</v>
@@ -38839,7 +38785,7 @@
         <v>56</v>
       </c>
       <c r="L52" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="M52">
         <v>5.008912564871331E-2</v>
@@ -38883,7 +38829,7 @@
         <v>56</v>
       </c>
       <c r="L53" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="M53">
         <v>5.830356212082257E-2</v>
@@ -38927,7 +38873,7 @@
         <v>34</v>
       </c>
       <c r="L54" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="M54">
         <v>3.848998337559708E-2</v>
@@ -38971,7 +38917,7 @@
         <v>34</v>
       </c>
       <c r="L55" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="M55">
         <v>3.7586318983874475E-2</v>
@@ -39015,7 +38961,7 @@
         <v>60</v>
       </c>
       <c r="L56" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="M56">
         <v>4.6813598676434483E-2</v>
@@ -39059,7 +39005,7 @@
         <v>60</v>
       </c>
       <c r="L57" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="M57">
         <v>5.9950274362933216E-2</v>
@@ -39103,7 +39049,7 @@
         <v>40</v>
       </c>
       <c r="L58" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="M58">
         <v>5.8189288278660045E-2</v>
@@ -39147,7 +39093,7 @@
         <v>40</v>
       </c>
       <c r="L59" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="M59">
         <v>5.427615192649405E-2</v>
@@ -39191,7 +39137,7 @@
         <v>58</v>
       </c>
       <c r="L60" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="M60">
         <v>4.2202311282246004E-2</v>
@@ -39235,7 +39181,7 @@
         <v>58</v>
       </c>
       <c r="L61" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="M61">
         <v>3.5851898318711939E-2</v>

</xml_diff>